<commit_message>
Testing cases for Newton-Raphson's method
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/NewtonRaphsonMinStepTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/NewtonRaphsonMinStepTest.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace-STS\maven.1536042399911\jacobi\src\test\resources\jacobi\test\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19065" windowHeight="2970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test f(x) = x^2 + y^2" sheetId="1" r:id="rId1"/>
-    <sheet name="test f(x) = (x - y)^2" sheetId="2" r:id="rId2"/>
+    <sheet name="test std normal dist 2D" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <oleSize ref="A1:P31"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>f(x)=</t>
   </si>
@@ -54,6 +58,18 @@
   </si>
   <si>
     <t>#100</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>z[i]z[j]</t>
+  </si>
+  <si>
+    <t>sig[i]sig[j]</t>
+  </si>
+  <si>
+    <t>Hessian=</t>
   </si>
 </sst>
 </file>
@@ -105,6 +121,1971 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>52387</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="618246" cy="289888"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="52387" y="1528762"/>
+              <a:ext cx="618246" cy="289888"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑧</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑢</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝜎</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="52387" y="1528762"/>
+              <a:ext cx="618246" cy="289888"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑧=(𝑥−𝑢)/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜎</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>71437</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1356462" cy="409920"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="71437" y="2262187"/>
+              <a:ext cx="1356462" cy="409920"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑓</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑋</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:sty m:val="p"/>
+                      </m:rPr>
+                      <a:rPr lang="en-HK" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>exp</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>⁡(−</m:t>
+                    </m:r>
+                    <m:nary>
+                      <m:naryPr>
+                        <m:chr m:val="∑"/>
+                        <m:subHide m:val="on"/>
+                        <m:supHide m:val="on"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:naryPr>
+                      <m:sub/>
+                      <m:sup/>
+                      <m:e>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑧</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑖</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>)</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:nary>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="71437" y="2262187"/>
+              <a:ext cx="1356462" cy="409920"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓(𝑋)=exp⁡(−∑▒〖〖𝑧_𝑖〗^2)〗</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3557589" cy="490538"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="3052762"/>
+              <a:ext cx="3557589" cy="490538"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1400" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1400" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1400" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1400" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=−2</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑧</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑖</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑧</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <m:rPr>
+                        <m:sty m:val="p"/>
+                      </m:rPr>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>exp</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>(−</m:t>
+                    </m:r>
+                    <m:nary>
+                      <m:naryPr>
+                        <m:chr m:val="∑"/>
+                        <m:subHide m:val="on"/>
+                        <m:supHide m:val="on"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:naryPr>
+                      <m:sub/>
+                      <m:sup/>
+                      <m:e>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                    <a:solidFill>
+                                      <a:schemeClr val="tx1"/>
+                                    </a:solidFill>
+                                    <a:effectLst/>
+                                    <a:latin typeface="+mn-lt"/>
+                                    <a:ea typeface="+mn-ea"/>
+                                    <a:cs typeface="+mn-cs"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                    <a:solidFill>
+                                      <a:schemeClr val="tx1"/>
+                                    </a:solidFill>
+                                    <a:effectLst/>
+                                    <a:latin typeface="+mn-lt"/>
+                                    <a:ea typeface="+mn-ea"/>
+                                    <a:cs typeface="+mn-cs"/>
+                                  </a:rPr>
+                                  <m:t>𝑧</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                    <a:solidFill>
+                                      <a:schemeClr val="tx1"/>
+                                    </a:solidFill>
+                                    <a:effectLst/>
+                                    <a:latin typeface="+mn-lt"/>
+                                    <a:ea typeface="+mn-ea"/>
+                                    <a:cs typeface="+mn-cs"/>
+                                  </a:rPr>
+                                  <m:t>𝑖</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>)</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:nary>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>−2</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑧</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝜎</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑓</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑋</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="3052762"/>
+              <a:ext cx="3557589" cy="490538"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑑</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑓</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>/(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑑</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> )</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=−2𝑧_𝑖  (𝑑𝑧_𝑖)/(𝑑𝑥_𝑖 )</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> exp(−∑▒〖〖𝑧_𝑖〗^2)〗</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>=(−2𝑧_𝑖)/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝜎</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>_𝑖  𝑓(𝑋)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4273413" cy="492955"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="4186237"/>
+              <a:ext cx="4273413" cy="492955"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1400" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1400" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑑</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑓</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1400" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1400" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1400" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑑𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑗</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−2</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑧</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜎</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑𝑓</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑗</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−2</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜎</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑧</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑑</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑗</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑓</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑋</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=2</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑓</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑋</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>[</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑧</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑧</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑗</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜎</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜎</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑗</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>,</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑗</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝜎</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑖</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="en-HK" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>]</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="4186237"/>
+              <a:ext cx="4273413" cy="492955"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑑</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>^</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>2 𝑓</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)/(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑑</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> 〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑑𝑥</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>〗_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑗</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> )</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=(−2𝑧_𝑖)/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜎_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖   𝑑𝑓/(𝑑𝑥_𝑗 )+(−2)/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜎_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖   (𝑑𝑧_𝑖)/(𝑑𝑥_𝑗 ) 𝑓(𝑋)=2𝑓(𝑋)[(2𝑧_𝑖 𝑧_𝑗)/(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜎_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖 </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜎_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑗 )−1_(𝑖,𝑗)/〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜎_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-HK" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖〗^2 ]</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -539,12 +2520,166 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.3</v>
+      </c>
+      <c r="B3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f>(A3-A7)/A8</f>
+        <v>0.3</v>
+      </c>
+      <c r="B11">
+        <f>(B3-B7)/B8</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f>EXP(-A11*A11-B11*B11)</f>
+        <v>0.55989836656540204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="50.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f>-2*A11*A14/A8</f>
+        <v>-0.33593901993924119</v>
+      </c>
+      <c r="B17">
+        <f>-2*B11*A14/B8</f>
+        <v>-0.78385771319156283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="54.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="array" ref="A21:B22">MMULT(TRANSPOSE(A11:B11),A11:B11)</f>
+        <v>0.09</v>
+      </c>
+      <c r="B21">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>0.21</v>
+      </c>
+      <c r="B22">
+        <v>0.48999999999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <f t="array" ref="A25:B26">MMULT(TRANSPOSE(A8:B8),A8:B8)</f>
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <f>2*$A$14*(2*A21/A25-1/A25)</f>
+        <v>-0.91823332116725942</v>
+      </c>
+      <c r="B29">
+        <f>2*$A$14*(2*B21/B25)</f>
+        <v>0.47031462791493772</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <f>2*$A$14*(2*A22/A26)</f>
+        <v>0.47031462791493772</v>
+      </c>
+      <c r="B30">
+        <f>2*$A$14*(2*B22/B26-1/B26)</f>
+        <v>-2.2395934662616225E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>